<commit_message>
Format dates and numbers
</commit_message>
<xml_diff>
--- a/spec/data/Spec.xlsx
+++ b/spec/data/Spec.xlsx
@@ -1,26 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView activeTab="4" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="257" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24740" windowHeight="13200" tabRatio="539"/>
   </bookViews>
   <sheets>
-    <sheet name="test_otros" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="test_spec" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="test_param" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Lenguajes" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="ont_demo" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="test_otros" sheetId="1" r:id="rId1"/>
+    <sheet name="test_spec" sheetId="2" r:id="rId2"/>
+    <sheet name="test_param" sheetId="3" r:id="rId3"/>
+    <sheet name="Lenguajes" sheetId="4" r:id="rId4"/>
+    <sheet name="ont_demo" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">test_param!$A$1:$L$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="Excel_BuiltIn__FilterDatabase" vbProcedure="false">test_spec!$A$1:$L$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">test_param!$A$1:$L$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_1" vbProcedure="false">test_param!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2">test_param!$A$1:$L$1</definedName>
+    <definedName name="_FilterDatabase_1" localSheetId="2">test_param!$A$1:$L$1</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase" localSheetId="2">test_spec!$A$1:$L$1</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -198,62 +201,58 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="0.00" numFmtId="165"/>
-    <numFmt formatCode="@" numFmtId="166"/>
-  </numFmts>
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
+      <b/>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
+      <b/>
       <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="10"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="00000000"/>
-      <sz val="10"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -265,72 +264,71 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left style="thick">
-        <color rgb="003C3C3C"/>
+        <color rgb="FF3C3C3C"/>
       </left>
       <right style="thick">
-        <color rgb="003C3C3C"/>
+        <color rgb="FF3C3C3C"/>
       </right>
       <top style="thick">
-        <color rgb="003C3C3C"/>
+        <color rgb="FF3C3C3C"/>
       </top>
       <bottom style="thick">
-        <color rgb="003C3C3C"/>
+        <color rgb="FF3C3C3C"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+  <cellStyleXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="166" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="11">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -389,52 +387,384 @@
       <rgbColor rgb="00993366"/>
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="003C3C3C"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IW7"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.3254901960784"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.7921568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.0117647058824"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="9.25882352941177"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="9.25882352941177"/>
+    <col min="1" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="4" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="257" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="1">
+    <row r="1" spans="1:6" ht="14.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="2">
+      <c r="B1" s="3">
+        <v>3.14</v>
+      </c>
+      <c r="C1" s="11">
+        <v>3</v>
+      </c>
+      <c r="D1" s="8">
+        <v>25569.041666666668</v>
+      </c>
+      <c r="E1" s="9">
+        <v>25569</v>
+      </c>
+      <c r="F1" s="10">
+        <v>3.4028236692093801E+38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="b">
-        <f aca="false">FALSE()</f>
+        <f>FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="3">
+    <row r="3" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -445,7 +775,7 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="4">
+    <row r="4" spans="1:6" ht="14.25" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -453,11 +783,11 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="b">
-        <f aca="false">FALSE()</f>
+        <f>FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="5">
+    <row r="5" spans="1:6" ht="14.25" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -465,11 +795,11 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="b">
-        <f aca="false">FALSE()</f>
+        <f>FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="6">
+    <row r="6" spans="1:6" ht="14.25" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -477,11 +807,11 @@
         <v>6</v>
       </c>
       <c r="C6" s="1" t="b">
-        <f aca="false">FALSE()</f>
+        <f>FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="7">
+    <row r="7" spans="1:6" ht="14.25" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -489,41 +819,35 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="b">
-        <f aca="false">FALSE()</f>
+        <f>FALSE()</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IW9"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B3" activeCellId="0" pane="topLeft" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.67058823529412"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="29.0274509803922"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.3725490196078"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="9.25882352941177"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="9.25882352941177"/>
+    <col min="1" max="257" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="1">
+    <row r="1" spans="1:3" ht="14.25" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
@@ -534,7 +858,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="2">
+    <row r="2" spans="1:3" ht="14.25" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
@@ -545,7 +869,7 @@
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="3">
+    <row r="3" spans="1:3" ht="14.25" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
@@ -556,7 +880,7 @@
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="4">
+    <row r="4" spans="1:3" ht="14.25" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
@@ -567,7 +891,7 @@
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="5">
+    <row r="5" spans="1:3" ht="14.25" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
@@ -578,7 +902,7 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="6">
+    <row r="6" spans="1:3" ht="14.25" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
@@ -589,7 +913,7 @@
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="7">
+    <row r="7" spans="1:3" ht="14.25" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -600,7 +924,7 @@
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="8">
+    <row r="8" spans="1:3" ht="14.25" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
@@ -611,7 +935,7 @@
         <v>24</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="9">
+    <row r="9" spans="1:3" ht="14.25" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
@@ -623,45 +947,28 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IW3"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.89411764705882"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.85490196078431"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.4"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.5803921568627"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.2509803921569"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.7882352941176"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.043137254902"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.1450980392157"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="14.1843137254902"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.38039215686275"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.23921568627451"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="14.7137254901961"/>
-    <col collapsed="false" hidden="false" max="257" min="13" style="1" width="9.25882352941177"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="9.25882352941177"/>
+    <col min="1" max="257" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="1">
+    <row r="1" spans="1:12" ht="14.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
@@ -699,7 +1006,7 @@
         <v>36</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="2">
+    <row r="2" spans="1:12" ht="14.25" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -719,7 +1026,7 @@
         <v>40</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.3" outlineLevel="0" r="3">
+    <row r="3" spans="1:12" ht="13.25" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>41</v>
       </c>
@@ -741,36 +1048,30 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:L1"/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IW2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E2" activeCellId="0" pane="topLeft" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.23921568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="2" style="1" width="4.70588235294118"/>
-    <col collapsed="false" hidden="false" max="257" min="6" style="1" width="9.25882352941177"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="9.25882352941177"/>
+    <col min="1" max="257" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="1">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="B1" s="2" t="s">
         <v>43</v>
       </c>
@@ -784,53 +1085,52 @@
         <v>46</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="2">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="1">
         <v>30</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C2" s="1">
         <v>50</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="1">
         <v>15</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="1">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK3"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C1" activeCellId="0" pane="topLeft" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.6078431372549"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="16.043137254902"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.2313725490196"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="9.18039215686274"/>
+    <col min="1" max="1025" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="1">
+    <row r="1" spans="1:4" ht="14">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -844,7 +1144,7 @@
         <v>49</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
+    <row r="2" spans="1:4" ht="14">
       <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
@@ -858,7 +1158,7 @@
         <v>52</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="3">
+    <row r="3" spans="1:4" ht="14">
       <c r="A3" s="1" t="s">
         <v>53</v>
       </c>
@@ -873,12 +1173,16 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix time precision (use decimal instead of float)
</commit_message>
<xml_diff>
--- a/spec/data/Spec.xlsx
+++ b/spec/data/Spec.xlsx
@@ -18,7 +18,7 @@
     <definedName name="_FilterDatabase_1" localSheetId="2">test_param!$A$1:$L$1</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase" localSheetId="2">test_spec!$A$1:$L$1</definedName>
   </definedNames>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -202,11 +202,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm"/>
-    <numFmt numFmtId="166" formatCode="&quot;USD&quot;\ 0"/>
+    <numFmt numFmtId="165" formatCode="&quot;USD&quot;\ 0"/>
+    <numFmt numFmtId="166" formatCode="[$-10409]m/d/yyyy\ h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -258,6 +259,11 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -267,7 +273,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -287,6 +293,21 @@
       </top>
       <bottom style="thick">
         <color rgb="FF3C3C3C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="9"/>
       </bottom>
       <diagonal/>
     </border>
@@ -317,12 +338,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -739,14 +763,14 @@
   <dimension ref="A1:IW7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="1"/>
     <col min="3" max="3" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" style="1" customWidth="1"/>
     <col min="5" max="257" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -757,16 +781,16 @@
       <c r="B1" s="3">
         <v>3.14</v>
       </c>
-      <c r="C1" s="11">
+      <c r="C1" s="10">
         <v>3</v>
       </c>
-      <c r="D1" s="8">
-        <v>25569.041666666668</v>
-      </c>
-      <c r="E1" s="9">
+      <c r="D1" s="13">
+        <v>41621.334004629629</v>
+      </c>
+      <c r="E1" s="8">
         <v>25569</v>
       </c>
-      <c r="F1" s="10">
+      <c r="F1" s="9">
         <v>3.4028236692093801E+38</v>
       </c>
     </row>
@@ -778,10 +802,10 @@
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="12">
         <v>3</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="11">
         <v>25569.041666666668</v>
       </c>
     </row>
@@ -863,7 +887,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="257" width="10.83203125" style="1"/>
   </cols>
@@ -984,7 +1008,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="257" width="10.83203125" style="1"/>
   </cols>
@@ -1087,7 +1111,7 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="257" width="10.83203125" style="1"/>
   </cols>
@@ -1146,12 +1170,12 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1025" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -1165,7 +1189,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
@@ -1179,7 +1203,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="14">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
Even more precise date times using Rational
</commit_message>
<xml_diff>
--- a/spec/data/Spec.xlsx
+++ b/spec/data/Spec.xlsx
@@ -312,8 +312,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -348,7 +350,7 @@
       <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -356,6 +358,7 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -363,6 +366,7 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -763,7 +767,7 @@
   <dimension ref="A1:IW7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -771,10 +775,12 @@
     <col min="1" max="2" width="10.83203125" style="1"/>
     <col min="3" max="3" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" style="1" customWidth="1"/>
-    <col min="5" max="257" width="10.83203125" style="1"/>
+    <col min="5" max="6" width="10.83203125" style="1"/>
+    <col min="7" max="7" width="17" style="1" customWidth="1"/>
+    <col min="8" max="257" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.25" customHeight="1">
+    <row r="1" spans="1:7" ht="14.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -793,8 +799,11 @@
       <c r="F1" s="9">
         <v>3.4028236692093801E+38</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="14.25" customHeight="1">
+      <c r="G1" s="13">
+        <v>42048.527835648143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -809,7 +818,7 @@
         <v>25569.041666666668</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.25" customHeight="1">
+    <row r="3" spans="1:7" ht="14.25" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -820,7 +829,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.25" customHeight="1">
+    <row r="4" spans="1:7" ht="14.25" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -832,7 +841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.25" customHeight="1">
+    <row r="5" spans="1:7" ht="14.25" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -844,7 +853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.25" customHeight="1">
+    <row r="6" spans="1:7" ht="14.25" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -856,7 +865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14.25" customHeight="1">
+    <row r="7" spans="1:7" ht="14.25" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Fix formatted shared strings (regressio in 1.7.0)
</commit_message>
<xml_diff>
--- a/spec/data/Spec.xlsx
+++ b/spec/data/Spec.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28615"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ebeigarts/code/saxlsx/spec/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24740" windowHeight="13200" tabRatio="539"/>
+    <workbookView xWindow="80" yWindow="440" windowWidth="24740" windowHeight="13200" tabRatio="539"/>
   </bookViews>
   <sheets>
     <sheet name="test_otros" sheetId="1" r:id="rId1"/>
@@ -18,8 +23,11 @@
     <definedName name="_FilterDatabase_1" localSheetId="2">test_param!$A$1:$L$1</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase" localSheetId="2">test_spec!$A$1:$L$1</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -30,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
   <si>
-    <t>LevenshteinDistance</t>
-  </si>
-  <si>
     <t>Case sensitive</t>
   </si>
   <si>
@@ -196,6 +201,22 @@
   </si>
   <si>
     <t>TST_ModMan_Insulto_SU_Normal</t>
+  </si>
+  <si>
+    <r>
+      <t>Levenshtein</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Distance</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -207,7 +228,7 @@
     <numFmt numFmtId="165" formatCode="&quot;USD&quot;\ 0"/>
     <numFmt numFmtId="166" formatCode="[$-10409]m/d/yyyy\ h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -263,6 +284,15 @@
       <sz val="8"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -439,6 +469,11 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -764,25 +799,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IW7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="1"/>
     <col min="3" max="3" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" style="1" customWidth="1"/>
     <col min="5" max="6" width="10.83203125" style="1"/>
     <col min="7" max="7" width="17" style="1" customWidth="1"/>
-    <col min="8" max="257" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.25" customHeight="1">
+    <row r="1" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="B1" s="3">
         <v>3.14</v>
@@ -803,9 +835,9 @@
         <v>42048.527835648143</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.25" customHeight="1">
+    <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="b">
         <f>FALSE()</f>
@@ -818,59 +850,59 @@
         <v>25569.041666666668</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.25" customHeight="1">
+    <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4" t="s">
+    </row>
+    <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A4" s="5" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="C4" s="1" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.25" customHeight="1">
+    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14.25" customHeight="1">
+    <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="14.25" customHeight="1">
+    <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1" t="b">
         <f>FALSE()</f>
@@ -880,268 +912,253 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IW9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="257" width="10.83203125" style="1"/>
+    <col min="1" max="3" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.25" customHeight="1">
+    <row r="1" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A2" s="5" t="s">
+      <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="6" t="s">
+    </row>
+    <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="6" t="s">
+    </row>
+    <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IW3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="257" width="10.83203125" style="1"/>
+    <col min="1" max="12" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.25" customHeight="1">
+    <row r="1" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:12" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="13.25" customHeight="1">
-      <c r="A3" s="5" t="s">
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="L3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:L1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IW2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="257" width="10.83203125" style="1"/>
+    <col min="1" max="5" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="B2" s="1">
         <v>30</v>
@@ -1163,67 +1180,62 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="10.83203125" style="1"/>
+    <col min="1" max="4" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1233,10 +1245,5 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>